<commit_message>
2.16 Commit: Complete subscribe. Can store and read subscriber data from the Excel file.
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -1,69 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yijiasun-my.sharepoint.com/personal/art_yijiasun_onmicrosoft_com/Documents/SDE/projects/weather-forecast-web-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_AD4DA82427541F7ACA7EB84F104B13206BE8DE12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5C21400-2303-43B5-9DE6-BD7D21F98C44}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_8237CF42D9D558428710DDB1A67ECEB30E22E7F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13D86FE1-A2F5-4854-9E05-43611A55B4CD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2736" yWindow="5880" windowWidth="16668" windowHeight="10488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="users" sheetId="1" r:id="rId1"/>
+    <sheet name="temp" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>address</t>
   </si>
   <si>
     <t>city</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Bellamy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sun</t>
   </si>
   <si>
     <t>michaelice2604@gmail.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Los Angeles</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>first name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>last name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yijia</t>
+  </si>
+  <si>
+    <t>931588213@qq.com</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Wu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	wurui9709@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,12 +85,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
       <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="等线"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,18 +111,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -392,57 +433,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="12.9140625" customWidth="1"/>
-    <col min="2" max="2" width="12.4140625" customWidth="1"/>
-    <col min="3" max="3" width="25.75" customWidth="1"/>
-    <col min="4" max="4" width="14.25" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A05C9E1D-30B6-40FA-BF21-D1DA693B8C6E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3.6 Commit: multiprocessing for web() and send_email(); send email at 6am in the timezone specifically for every single subscriber
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yijiasun-my.sharepoint.com/personal/art_yijiasun_onmicrosoft_com/Documents/SDE/projects/weather-forecast-web-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_8237CF42D9D558428710DDB1A67ECEB30E22E7F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13D86FE1-A2F5-4854-9E05-43611A55B4CD}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_8237532A873B0CB0EAE1E7F0A9CCC6F3293EEEE5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC176289-238D-4B99-89D8-D579B0581DD2}"/>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="5880" windowWidth="16668" windowHeight="10488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="3276" windowWidth="23040" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>firstname</t>
   </si>
@@ -35,6 +35,18 @@
     <t>city</t>
   </si>
   <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Wu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	wurui9709@gmail.com</t>
+  </si>
+  <si>
     <t>Bellamy</t>
   </si>
   <si>
@@ -42,34 +54,13 @@
   </si>
   <si>
     <t>michaelice2604@gmail.com</t>
-  </si>
-  <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
-    <t>Yijia</t>
-  </si>
-  <si>
-    <t>931588213@qq.com</t>
-  </si>
-  <si>
-    <t>Shanghai</t>
-  </si>
-  <si>
-    <t>Ryan</t>
-  </si>
-  <si>
-    <t>Wu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	wurui9709@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +85,16 @@
       <sz val="11"/>
       <name val="等线"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="等线"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="等线"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -103,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -141,16 +142,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -433,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -445,61 +482,21 @@
     <col min="3" max="3" width="10.109375" customWidth="1"/>
     <col min="4" max="4" width="26.44140625" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1"/>
+    <row r="1" spans="1:6">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -510,10 +507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -521,19 +518,57 @@
     <col min="3" max="3" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="G5" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
3.6 2nd Commit: avoid repeated subscriptions
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -1,110 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yijiasun-my.sharepoint.com/personal/art_yijiasun_onmicrosoft_com/Documents/SDE/projects/weather-forecast-web-app/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_8237532A873B0CB0EAE1E7F0A9CCC6F3293EEEE5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC176289-238D-4B99-89D8-D579B0581DD2}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="3276" windowWidth="23040" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="660" yWindow="3276" windowWidth="23040" windowHeight="12156" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="users" sheetId="1" r:id="rId1"/>
-    <sheet name="temp" sheetId="2" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="users" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="temp" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
-    <t>Ryan</t>
-  </si>
-  <si>
-    <t>Wu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	wurui9709@gmail.com</t>
-  </si>
-  <si>
-    <t>Bellamy</t>
-  </si>
-  <si>
-    <t>Sun</t>
-  </si>
-  <si>
-    <t>michaelice2604@gmail.com</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="7">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="3"/>
       <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="等线"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="等线"/>
     </font>
     <font>
-      <b/>
+      <name val="等线"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="等线"/>
     </font>
     <font>
-      <b/>
+      <name val="等线"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="等线"/>
     </font>
     <font>
-      <b/>
+      <name val="等线"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="等线"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -172,38 +132,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -469,109 +497,184 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col width="14.77734375" customWidth="1" min="2" max="2"/>
+    <col width="10.109375" customWidth="1" min="3" max="3"/>
+    <col width="26.44140625" customWidth="1" min="4" max="4"/>
+    <col width="15.33203125" customWidth="1" min="5" max="5"/>
+    <col width="12.6640625" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3"/>
+    <row r="1">
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>firstname</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>lastname</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>address</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>timezone</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Yijia</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>931588213@qq.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Shanghai</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col width="22.21875" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Ryan</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Wu</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	wurui9709@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>firstname</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>lastname</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>address</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="G2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="G5" s="1"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Bellamy</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>michaelice2604@gmail.com</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="G3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="G4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="G5" s="1" t="n"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3.7 1st Commit: only check if city and address are repeated
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yijiasun-my.sharepoint.com/personal/art_yijiasun_onmicrosoft_com/Documents/SDE/projects/weather-forecast-web-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_8237532A873B0BC22240FFF0A96B46773F5EEFC2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F06ADCB4-DAFD-443B-BDCA-378E5DFD0F43}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_8237532A873B0BC22240FFF0A96B46773F5EEFC2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D01C06E-DEEA-4DD7-A9D4-BFE32BE96537}"/>
   <bookViews>
     <workbookView xWindow="1356" yWindow="3048" windowWidth="23040" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>firstname</t>
   </si>
@@ -80,6 +80,10 @@
   </si>
   <si>
     <t>Los Angeles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jiangnan</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -458,7 +462,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -532,7 +536,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
3.9 7th Commit: unsubscribe
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1356" yWindow="3048" windowWidth="23040" windowHeight="12156" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9360" yWindow="6324" windowWidth="16488" windowHeight="9960" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="users" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="等线"/>
       <family val="2"/>
@@ -43,6 +43,11 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="等线"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -54,12 +59,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -102,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -111,6 +131,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -456,10 +479,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
@@ -472,34 +495,34 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>firstname</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>lastname</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>address</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>city</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>timezone</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -527,7 +550,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -555,7 +578,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -583,12 +606,12 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bellamy</t>
+          <t>Yijia</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -598,7 +621,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>michaelice2604@gmail.com</t>
+          <t>bellamy93158@gmail.com</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -609,6 +632,95 @@
       <c r="F5" t="n">
         <v>-8</v>
       </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Yijia</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>michaelice2604@gmail.com</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Shandong</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Yijia</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>michaelice2604@gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Yijia</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>michaelice2604@gmail.com</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Hongkong</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
3.13 3rd Commit: update the email sending logic
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yijiasun-my.sharepoint.com/personal/art_yijiasun_onmicrosoft_com/Documents/SDE/projects/weather-forecast-web-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_84EFA3EBE85517D8DD166453AA7F36B51A94C256" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E15399D-7715-41E4-B55B-4D0F29407647}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAD6225-6AC9-40C5-BC8A-FB8F545103F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>firstname</t>
   </si>
@@ -56,44 +56,57 @@
     <t>Null</t>
   </si>
   <si>
+    <t>Bellamy</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>michaelice2604@gmail.com</t>
+  </si>
+  <si>
+    <t>Yijia</t>
+  </si>
+  <si>
+    <t>yijiasun@qq.com</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>JiangNan</t>
+  </si>
+  <si>
+    <t>Cai</t>
+  </si>
+  <si>
+    <t>Art1st</t>
+  </si>
+  <si>
+    <t>bellamy93158@gmail.com</t>
+  </si>
+  <si>
+    <t>931588213@qq.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	wurui9709@gmail.com</t>
+  </si>
+  <si>
     <t>Jiangnan</t>
   </si>
   <si>
-    <t>Cai</t>
+    <t xml:space="preserve">	jiangnantsai404@gmail.com</t>
   </si>
   <si>
     <t>jiangnantsai404@gmail.com</t>
-  </si>
-  <si>
-    <t>Yijia</t>
-  </si>
-  <si>
-    <t>Sun</t>
-  </si>
-  <si>
-    <t>931588213@qq.com</t>
-  </si>
-  <si>
-    <t>Shanghai</t>
-  </si>
-  <si>
-    <t>Bellamy</t>
-  </si>
-  <si>
-    <t>michaelice2604@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	wurui9709@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	jiangnantsai404@gmail.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,14 +137,6 @@
       <name val="等线"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="等线"/>
@@ -234,9 +239,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -249,17 +253,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -540,41 +543,41 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="10.08203125" customWidth="1"/>
-    <col min="4" max="4" width="34.9140625" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="18.25" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -597,7 +600,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -620,20 +623,79 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6"/>
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>-7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="6"/>
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>-7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
@@ -641,7 +703,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -653,12 +715,12 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="18.4140625" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.4140625" customWidth="1"/>
-    <col min="10" max="10" width="29.75" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="10" max="10" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -686,13 +748,13 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
       </c>
       <c r="F2">
         <v>8</v>
@@ -709,7 +771,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -723,13 +785,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -743,13 +805,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>

</xml_diff>